<commit_message>
Updated set to better align with writing policy
</commit_message>
<xml_diff>
--- a/Backup Code/Megabots (Apple II)/MegaBots - Plan.xlsx
+++ b/Backup Code/Megabots (Apple II)/MegaBots - Plan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Dropbox\RetroArch\Achievements\Unwanted\Megabots (Apple II)\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Dropbox\RetroArch\Achievements\Megabots (Apple II)\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="65">
   <si>
     <t>Achievement Name</t>
   </si>
@@ -115,18 +115,6 @@
     <t>Clear level 1 with 150+ power credits</t>
   </si>
   <si>
-    <t>Clear level 4 in 10 steps or less [5 NS - 5 EW]</t>
-  </si>
-  <si>
-    <t>Clear level 3 in 10 steps or less [5 NS - 5 EW]</t>
-  </si>
-  <si>
-    <t>Clear level 2 in 10 steps or less [5 NS - 5 EW]</t>
-  </si>
-  <si>
-    <t>Clear level 1 in 10 steps or less [5 NS - 5 EW]</t>
-  </si>
-  <si>
     <t>Access all rooms in level 4</t>
   </si>
   <si>
@@ -172,9 +160,6 @@
     <t>Accumulate 230 power credits without an emergency recharge</t>
   </si>
   <si>
-    <t>Accumulate 500 power credits total before game's end</t>
-  </si>
-  <si>
     <t>Robot Reflexes</t>
   </si>
   <si>
@@ -190,15 +175,6 @@
     <t>XXXX4</t>
   </si>
   <si>
-    <t>Clear level 2 with 100+ power</t>
-  </si>
-  <si>
-    <t>Clear level 3 with 100+ power</t>
-  </si>
-  <si>
-    <t>Clear level 4 with 100+ power</t>
-  </si>
-  <si>
     <t>#</t>
   </si>
   <si>
@@ -217,19 +193,40 @@
     <t>Ready?</t>
   </si>
   <si>
-    <t>Defeat 3 monsters in a row without taking damage or an emergency recharge</t>
-  </si>
-  <si>
-    <t>Defeat 5 monsters in a row without taking damage or an emergency recharge</t>
-  </si>
-  <si>
-    <t>Defeat 10 monsters in a row without taking damage or an emergency recharge</t>
-  </si>
-  <si>
     <t>Accumulate 350 power credits</t>
   </si>
   <si>
     <t>Accumulate 500 power credits</t>
+  </si>
+  <si>
+    <t>Clear level 1 in 10 steps or less</t>
+  </si>
+  <si>
+    <t>Clear level 2 in 10 steps or less</t>
+  </si>
+  <si>
+    <t>Clear level 3 in 10 steps or less</t>
+  </si>
+  <si>
+    <t>Clear level 4 in 10 steps or less</t>
+  </si>
+  <si>
+    <t>Defeat 3 bad robots in a row without taking damage or an emergency recharge, shooting good robots does not add to count</t>
+  </si>
+  <si>
+    <t>Defeat 5 bad robots in a row without taking damage or an emergency recharge, shooting good robots does not add to count</t>
+  </si>
+  <si>
+    <t>Defeat 10 bad robots in a row without taking damage or an emergency recharge, shooting good robots does not add to count</t>
+  </si>
+  <si>
+    <t>Clear level 2 with 100+ power credits</t>
+  </si>
+  <si>
+    <t>Clear level 3 with 100+ power credits</t>
+  </si>
+  <si>
+    <t>Clear level 4 with 100+ power credits</t>
   </si>
 </sst>
 </file>
@@ -594,8 +591,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,7 +633,7 @@
         <v>73134</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D2" s="3">
         <v>10</v>
@@ -653,7 +650,7 @@
         <v>73135</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D3" s="3">
         <v>10</v>
@@ -670,7 +667,7 @@
         <v>73136</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D4" s="3">
         <v>10</v>
@@ -687,7 +684,7 @@
         <v>73137</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D5" s="3">
         <v>10</v>
@@ -710,7 +707,7 @@
         <v>10</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="3" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -727,7 +724,7 @@
         <v>10</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="3" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -744,7 +741,7 @@
         <v>10</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="10" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -773,13 +770,13 @@
         <v>73146</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D10" s="3">
         <v>10</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="3" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -796,7 +793,7 @@
         <v>10</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="3" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -813,7 +810,7 @@
         <v>10</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="3" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -830,7 +827,7 @@
         <v>10</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="3" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -847,7 +844,7 @@
         <v>25</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="3" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -864,7 +861,7 @@
         <v>25</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="3" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -881,7 +878,7 @@
         <v>25</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="3" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -898,7 +895,7 @@
         <v>25</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="3" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -915,7 +912,7 @@
         <v>10</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="3" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -932,7 +929,7 @@
         <v>10</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="3" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -949,7 +946,7 @@
         <v>25</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="3" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -966,7 +963,7 @@
         <v>25</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="3" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -974,16 +971,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D22" s="3">
         <v>5</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="3" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -991,16 +988,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D23" s="3">
         <v>5</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:6" s="3" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -1008,16 +1005,16 @@
         <v>23</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D24" s="3">
         <v>10</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="3" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -1025,16 +1022,16 @@
         <v>24</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D25" s="3">
         <v>25</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="3" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -1762,19 +1759,19 @@
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="str">
         <f>"[ach="&amp;Achievements!B6&amp;"] "&amp;Achievements!C6&amp;" ("&amp;Achievements!D6&amp;") - "&amp;Achievements!E6</f>
-        <v>[ach=73138] Taste of Power (10) - Clear level 4 with 100+ power</v>
+        <v>[ach=73138] Taste of Power (10) - Clear level 4 with 100+ power credits</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="str">
         <f>"[ach="&amp;Achievements!B7&amp;"] "&amp;Achievements!C7&amp;" ("&amp;Achievements!D7&amp;") - "&amp;Achievements!E7</f>
-        <v>[ach=73139] Hour of Power (10) - Clear level 3 with 100+ power</v>
+        <v>[ach=73139] Hour of Power (10) - Clear level 3 with 100+ power credits</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="str">
         <f>"[ach="&amp;Achievements!B8&amp;"] "&amp;Achievements!C8&amp;" ("&amp;Achievements!D8&amp;") - "&amp;Achievements!E8</f>
-        <v>[ach=73140] Powered Armor (10) - Clear level 2 with 100+ power</v>
+        <v>[ach=73140] Powered Armor (10) - Clear level 2 with 100+ power credits</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
@@ -1786,25 +1783,25 @@
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="str">
         <f>"[ach="&amp;Achievements!B10&amp;"] "&amp;Achievements!C10&amp;" ("&amp;Achievements!D10&amp;") - "&amp;Achievements!E10</f>
-        <v>[ach=73146] Logic Gate Analysis (10) - Clear level 4 in 10 steps or less [5 NS - 5 EW]</v>
+        <v>[ach=73146] Logic Gate Analysis (10) - Clear level 4 in 10 steps or less</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="str">
         <f>"[ach="&amp;Achievements!B11&amp;"] "&amp;Achievements!C11&amp;" ("&amp;Achievements!D11&amp;") - "&amp;Achievements!E11</f>
-        <v>[ach=73147] Elimination Grid (10) - Clear level 3 in 10 steps or less [5 NS - 5 EW]</v>
+        <v>[ach=73147] Elimination Grid (10) - Clear level 3 in 10 steps or less</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="str">
         <f>"[ach="&amp;Achievements!B12&amp;"] "&amp;Achievements!C12&amp;" ("&amp;Achievements!D12&amp;") - "&amp;Achievements!E12</f>
-        <v>[ach=73148] Ockham's Razor (10) - Clear level 2 in 10 steps or less [5 NS - 5 EW]</v>
+        <v>[ach=73148] Ockham's Razor (10) - Clear level 2 in 10 steps or less</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="str">
         <f>"[ach="&amp;Achievements!B13&amp;"] "&amp;Achievements!C13&amp;" ("&amp;Achievements!D13&amp;") - "&amp;Achievements!E13</f>
-        <v>[ach=73149] Mastermind (10) - Clear level 1 in 10 steps or less [5 NS - 5 EW]</v>
+        <v>[ach=73149] Mastermind (10) - Clear level 1 in 10 steps or less</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
@@ -1864,19 +1861,19 @@
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="str">
         <f>"[ach="&amp;Achievements!B23&amp;"] "&amp;Achievements!C23&amp;" ("&amp;Achievements!D23&amp;") - "&amp;Achievements!E23</f>
-        <v>[ach=XXXX2] Quick Draw (5) - Defeat 3 monsters in a row without taking damage or an emergency recharge</v>
+        <v>[ach=XXXX2] Quick Draw (5) - Defeat 3 bad robots in a row without taking damage or an emergency recharge, shooting good robots does not add to count</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="str">
         <f>"[ach="&amp;Achievements!B24&amp;"] "&amp;Achievements!C24&amp;" ("&amp;Achievements!D24&amp;") - "&amp;Achievements!E24</f>
-        <v>[ach=XXXX3] Robot Reflexes (10) - Defeat 5 monsters in a row without taking damage or an emergency recharge</v>
+        <v>[ach=XXXX3] Robot Reflexes (10) - Defeat 5 bad robots in a row without taking damage or an emergency recharge, shooting good robots does not add to count</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="str">
         <f>"[ach="&amp;Achievements!B25&amp;"] "&amp;Achievements!C25&amp;" ("&amp;Achievements!D25&amp;") - "&amp;Achievements!E25</f>
-        <v>[ach=XXXX4] Quickest Gun on the Grid (25) - Defeat 10 monsters in a row without taking damage or an emergency recharge</v>
+        <v>[ach=XXXX4] Quickest Gun on the Grid (25) - Defeat 10 bad robots in a row without taking damage or an emergency recharge, shooting good robots does not add to count</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
@@ -1930,19 +1927,19 @@
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="str">
         <f>"title = "&amp;CHAR(34)&amp;Achievements!C6&amp;CHAR(34)&amp;", description = "&amp;CHAR(34)&amp;Achievements!E6&amp;CHAR(34)&amp;", points = "&amp;Achievements!D6&amp;", id = " &amp;Achievements!B6&amp;","</f>
-        <v>title = "Taste of Power", description = "Clear level 4 with 100+ power", points = 10, id = 73138,</v>
+        <v>title = "Taste of Power", description = "Clear level 4 with 100+ power credits", points = 10, id = 73138,</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="str">
         <f>"title = "&amp;CHAR(34)&amp;Achievements!C7&amp;CHAR(34)&amp;", description = "&amp;CHAR(34)&amp;Achievements!E7&amp;CHAR(34)&amp;", points = "&amp;Achievements!D7&amp;", id = " &amp;Achievements!B7&amp;","</f>
-        <v>title = "Hour of Power", description = "Clear level 3 with 100+ power", points = 10, id = 73139,</v>
+        <v>title = "Hour of Power", description = "Clear level 3 with 100+ power credits", points = 10, id = 73139,</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="str">
         <f>"title = "&amp;CHAR(34)&amp;Achievements!C8&amp;CHAR(34)&amp;", description = "&amp;CHAR(34)&amp;Achievements!E8&amp;CHAR(34)&amp;", points = "&amp;Achievements!D8&amp;", id = " &amp;Achievements!B8&amp;","</f>
-        <v>title = "Powered Armor", description = "Clear level 2 with 100+ power", points = 10, id = 73140,</v>
+        <v>title = "Powered Armor", description = "Clear level 2 with 100+ power credits", points = 10, id = 73140,</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
@@ -1954,25 +1951,25 @@
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="str">
         <f>"title = "&amp;CHAR(34)&amp;Achievements!C10&amp;CHAR(34)&amp;", description = "&amp;CHAR(34)&amp;Achievements!E10&amp;CHAR(34)&amp;", points = "&amp;Achievements!D10&amp;", id = " &amp;Achievements!B10&amp;","</f>
-        <v>title = "Logic Gate Analysis", description = "Clear level 4 in 10 steps or less [5 NS - 5 EW]", points = 10, id = 73146,</v>
+        <v>title = "Logic Gate Analysis", description = "Clear level 4 in 10 steps or less", points = 10, id = 73146,</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="str">
         <f>"title = "&amp;CHAR(34)&amp;Achievements!C11&amp;CHAR(34)&amp;", description = "&amp;CHAR(34)&amp;Achievements!E11&amp;CHAR(34)&amp;", points = "&amp;Achievements!D11&amp;", id = " &amp;Achievements!B11&amp;","</f>
-        <v>title = "Elimination Grid", description = "Clear level 3 in 10 steps or less [5 NS - 5 EW]", points = 10, id = 73147,</v>
+        <v>title = "Elimination Grid", description = "Clear level 3 in 10 steps or less", points = 10, id = 73147,</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="str">
         <f>"title = "&amp;CHAR(34)&amp;Achievements!C12&amp;CHAR(34)&amp;", description = "&amp;CHAR(34)&amp;Achievements!E12&amp;CHAR(34)&amp;", points = "&amp;Achievements!D12&amp;", id = " &amp;Achievements!B12&amp;","</f>
-        <v>title = "Ockham's Razor", description = "Clear level 2 in 10 steps or less [5 NS - 5 EW]", points = 10, id = 73148,</v>
+        <v>title = "Ockham's Razor", description = "Clear level 2 in 10 steps or less", points = 10, id = 73148,</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="str">
         <f>"title = "&amp;CHAR(34)&amp;Achievements!C13&amp;CHAR(34)&amp;", description = "&amp;CHAR(34)&amp;Achievements!E13&amp;CHAR(34)&amp;", points = "&amp;Achievements!D13&amp;", id = " &amp;Achievements!B13&amp;","</f>
-        <v>title = "Mastermind", description = "Clear level 1 in 10 steps or less [5 NS - 5 EW]", points = 10, id = 73149,</v>
+        <v>title = "Mastermind", description = "Clear level 1 in 10 steps or less", points = 10, id = 73149,</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
@@ -2032,19 +2029,19 @@
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="str">
         <f>"title = "&amp;CHAR(34)&amp;Achievements!C23&amp;CHAR(34)&amp;", description = "&amp;CHAR(34)&amp;Achievements!E23&amp;CHAR(34)&amp;", points = "&amp;Achievements!D23&amp;", id = " &amp;Achievements!B23&amp;","</f>
-        <v>title = "Quick Draw", description = "Defeat 3 monsters in a row without taking damage or an emergency recharge", points = 5, id = XXXX2,</v>
+        <v>title = "Quick Draw", description = "Defeat 3 bad robots in a row without taking damage or an emergency recharge, shooting good robots does not add to count", points = 5, id = XXXX2,</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="str">
         <f>"title = "&amp;CHAR(34)&amp;Achievements!C24&amp;CHAR(34)&amp;", description = "&amp;CHAR(34)&amp;Achievements!E24&amp;CHAR(34)&amp;", points = "&amp;Achievements!D24&amp;", id = " &amp;Achievements!B24&amp;","</f>
-        <v>title = "Robot Reflexes", description = "Defeat 5 monsters in a row without taking damage or an emergency recharge", points = 10, id = XXXX3,</v>
+        <v>title = "Robot Reflexes", description = "Defeat 5 bad robots in a row without taking damage or an emergency recharge, shooting good robots does not add to count", points = 10, id = XXXX3,</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="str">
         <f>"title = "&amp;CHAR(34)&amp;Achievements!C25&amp;CHAR(34)&amp;", description = "&amp;CHAR(34)&amp;Achievements!E25&amp;CHAR(34)&amp;", points = "&amp;Achievements!D25&amp;", id = " &amp;Achievements!B25&amp;","</f>
-        <v>title = "Quickest Gun on the Grid", description = "Defeat 10 monsters in a row without taking damage or an emergency recharge", points = 25, id = XXXX4,</v>
+        <v>title = "Quickest Gun on the Grid", description = "Defeat 10 bad robots in a row without taking damage or an emergency recharge, shooting good robots does not add to count", points = 25, id = XXXX4,</v>
       </c>
     </row>
   </sheetData>
@@ -2072,7 +2069,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>0</v>
@@ -2081,22 +2078,22 @@
         <v>1</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2242,7 +2239,7 @@
       </c>
       <c r="C6" s="5" t="str">
         <f>Achievements!E6</f>
-        <v>Clear level 4 with 100+ power</v>
+        <v>Clear level 4 with 100+ power credits</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>4</v>
@@ -2275,7 +2272,7 @@
       </c>
       <c r="C7" s="5" t="str">
         <f>Achievements!E7</f>
-        <v>Clear level 3 with 100+ power</v>
+        <v>Clear level 3 with 100+ power credits</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>4</v>
@@ -2308,7 +2305,7 @@
       </c>
       <c r="C8" s="5" t="str">
         <f>Achievements!E8</f>
-        <v>Clear level 2 with 100+ power</v>
+        <v>Clear level 2 with 100+ power credits</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>4</v>
@@ -2374,7 +2371,7 @@
       </c>
       <c r="C10" s="5" t="str">
         <f>Achievements!E10</f>
-        <v>Clear level 4 in 10 steps or less [5 NS - 5 EW]</v>
+        <v>Clear level 4 in 10 steps or less</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>4</v>
@@ -2407,7 +2404,7 @@
       </c>
       <c r="C11" s="5" t="str">
         <f>Achievements!E11</f>
-        <v>Clear level 3 in 10 steps or less [5 NS - 5 EW]</v>
+        <v>Clear level 3 in 10 steps or less</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>4</v>
@@ -2440,7 +2437,7 @@
       </c>
       <c r="C12" s="5" t="str">
         <f>Achievements!E12</f>
-        <v>Clear level 2 in 10 steps or less [5 NS - 5 EW]</v>
+        <v>Clear level 2 in 10 steps or less</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>4</v>
@@ -2473,7 +2470,7 @@
       </c>
       <c r="C13" s="5" t="str">
         <f>Achievements!E13</f>
-        <v>Clear level 1 in 10 steps or less [5 NS - 5 EW]</v>
+        <v>Clear level 1 in 10 steps or less</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>4</v>
@@ -2803,7 +2800,7 @@
       </c>
       <c r="C23" s="5" t="str">
         <f>Achievements!E23</f>
-        <v>Defeat 3 monsters in a row without taking damage or an emergency recharge</v>
+        <v>Defeat 3 bad robots in a row without taking damage or an emergency recharge, shooting good robots does not add to count</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>4</v>
@@ -2836,7 +2833,7 @@
       </c>
       <c r="C24" s="5" t="str">
         <f>Achievements!E24</f>
-        <v>Defeat 5 monsters in a row without taking damage or an emergency recharge</v>
+        <v>Defeat 5 bad robots in a row without taking damage or an emergency recharge, shooting good robots does not add to count</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>4</v>
@@ -2869,7 +2866,7 @@
       </c>
       <c r="C25" s="5" t="str">
         <f>Achievements!E25</f>
-        <v>Defeat 10 monsters in a row without taking damage or an emergency recharge</v>
+        <v>Defeat 10 bad robots in a row without taking damage or an emergency recharge, shooting good robots does not add to count</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>4</v>

</xml_diff>